<commit_message>
Added M51134 for all of the bass.
</commit_message>
<xml_diff>
--- a/Data/ICs.xlsx
+++ b/Data/ICs.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13830" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13830"/>
   </bookViews>
   <sheets>
     <sheet name="Linear" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="278">
   <si>
     <t>Part Number</t>
   </si>
@@ -808,13 +808,61 @@
   </si>
   <si>
     <t>MCU-0003</t>
+  </si>
+  <si>
+    <t>LINEAR-0038</t>
+  </si>
+  <si>
+    <t>Bass Enhancer</t>
+  </si>
+  <si>
+    <t>M51134</t>
+  </si>
+  <si>
+    <t>7-15V, 4.5-5.5V</t>
+  </si>
+  <si>
+    <t>5V regulator, Opamp, VCA</t>
+  </si>
+  <si>
+    <t>Sub-harmonic synthesizer for Bass Enhancement</t>
+  </si>
+  <si>
+    <t>M51134P</t>
+  </si>
+  <si>
+    <t>DIP-20</t>
+  </si>
+  <si>
+    <t>Mitsubishi</t>
+  </si>
+  <si>
+    <t>Small Bear Electronics</t>
+  </si>
+  <si>
+    <t>Footprint Ref 1</t>
+  </si>
+  <si>
+    <t>Footprint Path 1</t>
+  </si>
+  <si>
+    <t>Footprint Ref 2</t>
+  </si>
+  <si>
+    <t>Footprint Path 2</t>
+  </si>
+  <si>
+    <t>DIP-8</t>
+  </si>
+  <si>
+    <t>DIP-14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -824,14 +872,23 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -860,7 +917,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -870,6 +927,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1178,10 +1237,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD38"/>
+  <dimension ref="A1:AF39"/>
   <sheetViews>
-    <sheetView topLeftCell="F4" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7:L39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1195,18 +1254,19 @@
     <col min="8" max="8" width="34.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="27" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.7109375" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="27" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1232,58 +1292,64 @@
         <v>5</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>6</v>
+        <v>272</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>7</v>
+        <v>273</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
         <v>199</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>200</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>201</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>202</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>13</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
         <v>14</v>
       </c>
-      <c r="V1" t="s">
+      <c r="X1" t="s">
         <v>203</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>204</v>
       </c>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
       <c r="AA1" s="2"/>
       <c r="AB1" s="2"/>
       <c r="AC1" s="2"/>
       <c r="AD1" s="2"/>
-    </row>
-    <row r="2" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+    </row>
+    <row r="2" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1314,35 +1380,41 @@
       <c r="J2" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K2" t="b">
-        <v>0</v>
-      </c>
-      <c r="L2" s="6" t="s">
+      <c r="K2" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="M2" t="b">
+        <v>0</v>
+      </c>
+      <c r="N2" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="M2" s="6" t="s">
+      <c r="O2" s="6" t="s">
         <v>217</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>218</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>219</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="T2" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="3" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>106</v>
       </c>
@@ -1373,35 +1445,41 @@
       <c r="J3" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K3" t="b">
-        <v>0</v>
-      </c>
-      <c r="L3" s="6" t="s">
+      <c r="K3" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="M3" t="b">
+        <v>0</v>
+      </c>
+      <c r="N3" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>225</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>226</v>
       </c>
-      <c r="P3" s="6" t="s">
+      <c r="R3" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>227</v>
       </c>
-      <c r="R3" s="6" t="s">
+      <c r="T3" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>107</v>
       </c>
@@ -1432,35 +1510,41 @@
       <c r="J4" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K4" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6" t="s">
+      <c r="K4" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="M4" t="b">
+        <v>0</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="M4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>238</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="Q4" s="6" t="s">
         <v>239</v>
       </c>
-      <c r="P4" s="6" t="s">
+      <c r="R4" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>240</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="T4" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="U4" s="6" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>108</v>
       </c>
@@ -1491,35 +1575,41 @@
       <c r="J5" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K5" t="b">
-        <v>0</v>
-      </c>
-      <c r="L5" s="6" t="s">
+      <c r="K5" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="M5" t="b">
+        <v>0</v>
+      </c>
+      <c r="N5" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="M5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>242</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="Q5" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="R5" s="6" t="s">
         <v>244</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="S5" s="6" t="s">
         <v>245</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="T5" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="U5" s="6" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>109</v>
       </c>
@@ -1550,35 +1640,41 @@
       <c r="J6" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K6" t="b">
-        <v>0</v>
-      </c>
-      <c r="L6" s="6" t="s">
+      <c r="K6" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="M6" t="b">
+        <v>0</v>
+      </c>
+      <c r="N6" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="M6" s="6" t="s">
+      <c r="O6" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="N6" s="6" t="s">
+      <c r="P6" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="Q6" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="P6" s="6" t="s">
+      <c r="R6" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="S6" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="R6" s="6" t="s">
+      <c r="T6" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="U6" s="6" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>110</v>
       </c>
@@ -1603,15 +1699,17 @@
       <c r="J7" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K7" t="b">
-        <v>0</v>
-      </c>
-      <c r="L7" s="6"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" t="b">
+        <v>0</v>
+      </c>
       <c r="N7" s="6"/>
       <c r="P7" s="6"/>
       <c r="R7" s="6"/>
-    </row>
-    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T7" s="6"/>
+    </row>
+    <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>111</v>
       </c>
@@ -1636,15 +1734,17 @@
       <c r="J8" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K8" t="b">
-        <v>0</v>
-      </c>
-      <c r="L8" s="6"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" t="b">
+        <v>0</v>
+      </c>
       <c r="N8" s="6"/>
       <c r="P8" s="6"/>
       <c r="R8" s="6"/>
-    </row>
-    <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="T8" s="6"/>
+    </row>
+    <row r="9" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>112</v>
       </c>
@@ -1675,35 +1775,37 @@
       <c r="J9" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K9" t="b">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3" t="s">
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" t="b">
+        <v>0</v>
+      </c>
+      <c r="N9" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="M9" s="3" t="s">
+      <c r="O9" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="N9" s="3" t="s">
+      <c r="P9" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="Q9" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="P9" s="6" t="s">
+      <c r="R9" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="Q9" s="6" t="s">
+      <c r="S9" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="R9" s="6" t="s">
+      <c r="T9" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="S9" s="6" t="s">
+      <c r="U9" s="6" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>113</v>
       </c>
@@ -1734,35 +1836,37 @@
       <c r="J10" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K10" t="b">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3" t="s">
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" t="b">
+        <v>0</v>
+      </c>
+      <c r="N10" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="M10" s="3" t="s">
+      <c r="O10" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="P10" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="Q10" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="P10" s="3" t="s">
+      <c r="R10" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="Q10" s="3" t="s">
+      <c r="S10" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="R10" s="3" t="s">
+      <c r="T10" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="S10" s="3" t="s">
+      <c r="U10" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>114</v>
       </c>
@@ -1786,11 +1890,13 @@
       <c r="J11" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>115</v>
       </c>
@@ -1811,11 +1917,13 @@
       <c r="J12" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K12" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>116</v>
       </c>
@@ -1834,11 +1942,13 @@
       <c r="J13" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K13" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>117</v>
       </c>
@@ -1859,11 +1969,13 @@
       <c r="J14" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>118</v>
       </c>
@@ -1884,11 +1996,13 @@
       <c r="J15" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+      <c r="M15" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>119</v>
       </c>
@@ -1909,11 +2023,13 @@
       <c r="J16" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>251</v>
       </c>
@@ -1944,23 +2060,25 @@
       <c r="J17" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K17" t="b">
-        <v>0</v>
-      </c>
-      <c r="L17" s="3" t="s">
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" t="b">
+        <v>0</v>
+      </c>
+      <c r="N17" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="M17" s="3" t="s">
+      <c r="O17" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="N17" s="3" t="s">
+      <c r="P17" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="Q17" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="18" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>252</v>
       </c>
@@ -1979,11 +2097,13 @@
       <c r="J18" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K18" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>120</v>
       </c>
@@ -2004,11 +2124,13 @@
       <c r="J19" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K19" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>121</v>
       </c>
@@ -2027,11 +2149,13 @@
       <c r="J20" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>122</v>
       </c>
@@ -2050,11 +2174,13 @@
       <c r="J21" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K21" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+      <c r="M21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>123</v>
       </c>
@@ -2073,11 +2199,13 @@
       <c r="J22" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K22" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+      <c r="M22" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>124</v>
       </c>
@@ -2098,11 +2226,13 @@
       <c r="J23" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K23" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+      <c r="M23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>125</v>
       </c>
@@ -2123,11 +2253,13 @@
       <c r="J24" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K24" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>126</v>
       </c>
@@ -2148,11 +2280,13 @@
       <c r="J25" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K25" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+      <c r="M25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>127</v>
       </c>
@@ -2171,11 +2305,13 @@
       <c r="J26" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K26" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>128</v>
       </c>
@@ -2196,11 +2332,13 @@
       <c r="J27" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K27" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+      <c r="M27" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>129</v>
       </c>
@@ -2221,11 +2359,13 @@
       <c r="J28" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K28" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>130</v>
       </c>
@@ -2244,11 +2384,13 @@
       <c r="J29" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>131</v>
       </c>
@@ -2267,11 +2409,13 @@
       <c r="J30" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K30" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>132</v>
       </c>
@@ -2292,11 +2436,13 @@
       <c r="J31" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K31" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+      <c r="M31" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>133</v>
       </c>
@@ -2317,11 +2463,13 @@
       <c r="J32" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K32" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>193</v>
       </c>
@@ -2342,11 +2490,13 @@
       <c r="J33" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K33" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>194</v>
       </c>
@@ -2367,11 +2517,13 @@
       <c r="J34" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K34" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>195</v>
       </c>
@@ -2390,11 +2542,13 @@
       <c r="J35" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K35" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>253</v>
       </c>
@@ -2425,23 +2579,23 @@
       <c r="J36" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K36" t="b">
-        <v>0</v>
-      </c>
-      <c r="L36" s="3" t="s">
+      <c r="M36" t="b">
+        <v>0</v>
+      </c>
+      <c r="N36" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="M36" s="3" t="s">
+      <c r="O36" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="N36" s="3" t="s">
+      <c r="P36" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="O36" s="3" t="s">
+      <c r="Q36" s="3" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:15" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:17" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>254</v>
       </c>
@@ -2472,23 +2626,23 @@
       <c r="J37" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K37" t="b">
-        <v>0</v>
-      </c>
-      <c r="L37" s="3" t="s">
+      <c r="M37" t="b">
+        <v>0</v>
+      </c>
+      <c r="N37" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="M37" s="3" t="s">
+      <c r="O37" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="N37" s="3" t="s">
+      <c r="P37" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="O37" s="3" t="s">
+      <c r="Q37" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="38" spans="1:15" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:17" s="3" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>255</v>
       </c>
@@ -2519,20 +2673,70 @@
       <c r="J38" s="3" t="s">
         <v>257</v>
       </c>
-      <c r="K38" t="b">
-        <v>0</v>
-      </c>
-      <c r="L38" s="3" t="s">
+      <c r="K38" s="10"/>
+      <c r="M38" t="b">
+        <v>0</v>
+      </c>
+      <c r="N38" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="M38" s="3" t="s">
+      <c r="O38" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="N38" s="3" t="s">
+      <c r="P38" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="O38" s="3" t="s">
+      <c r="Q38" s="3" t="s">
         <v>166</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="B39" t="s">
+        <v>263</v>
+      </c>
+      <c r="C39" t="s">
+        <v>264</v>
+      </c>
+      <c r="D39" t="s">
+        <v>265</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="I39" t="s">
+        <v>269</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" t="b">
+        <v>0</v>
+      </c>
+      <c r="N39" t="s">
+        <v>270</v>
+      </c>
+      <c r="O39" t="s">
+        <v>268</v>
+      </c>
+      <c r="P39" t="s">
+        <v>271</v>
+      </c>
+      <c r="Q39">
+        <v>1539</v>
       </c>
     </row>
   </sheetData>
@@ -2883,7 +3087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>